<commit_message>
working on assignment1 report.
</commit_message>
<xml_diff>
--- a/Assignment1/Assignment_1_result_plot_Kazumi.xlsx
+++ b/Assignment1/Assignment_1_result_plot_Kazumi.xlsx
@@ -270,16 +270,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -369,7 +369,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -703,11 +702,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2102070584"/>
-        <c:axId val="2115057240"/>
+        <c:axId val="2073880584"/>
+        <c:axId val="2073927832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2102070584"/>
+        <c:axId val="2073880584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -729,13 +728,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115057240"/>
+        <c:crossAx val="2073927832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -743,7 +741,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115057240"/>
+        <c:axId val="2073927832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -766,21 +764,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2102070584"/>
+        <c:crossAx val="2073880584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -843,7 +839,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.094719474168293"/>
           <c:y val="0.0338101430429129"/>
-          <c:w val="0.736490791215201"/>
+          <c:w val="0.611660380986976"/>
           <c:h val="0.852553372310906"/>
         </c:manualLayout>
       </c:layout>
@@ -1324,11 +1320,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2115431832"/>
-        <c:axId val="2115434808"/>
+        <c:axId val="2079131448"/>
+        <c:axId val="2079122552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2115431832"/>
+        <c:axId val="2079131448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1337,7 +1333,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115434808"/>
+        <c:crossAx val="2079122552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1345,7 +1341,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115434808"/>
+        <c:axId val="2079122552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1375,14 +1371,23 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115431832"/>
+        <c:crossAx val="2079131448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.75033921302578"/>
+          <c:y val="0.307004509051753"/>
+          <c:w val="0.238805970149254"/>
+          <c:h val="0.428970224875737"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1927,11 +1932,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2115828440"/>
-        <c:axId val="2115831416"/>
+        <c:axId val="2112909032"/>
+        <c:axId val="2112912008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2115828440"/>
+        <c:axId val="2112909032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1940,7 +1945,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115831416"/>
+        <c:crossAx val="2112912008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1948,7 +1953,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115831416"/>
+        <c:axId val="2112912008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1959,7 +1964,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115828440"/>
+        <c:crossAx val="2112909032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2279,11 +2284,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2115866072"/>
-        <c:axId val="2115869192"/>
+        <c:axId val="2113897240"/>
+        <c:axId val="2113900360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2115866072"/>
+        <c:axId val="2113897240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2292,7 +2297,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115869192"/>
+        <c:crossAx val="2113900360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2300,7 +2305,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115869192"/>
+        <c:axId val="2113900360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2311,7 +2316,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115866072"/>
+        <c:crossAx val="2113897240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2378,8 +2383,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>723900</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>120650</xdr:rowOff>
     </xdr:to>
@@ -2958,8 +2963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A22:D54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
+      <selection activeCell="V34" sqref="V34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2970,25 +2975,25 @@
   </cols>
   <sheetData>
     <row r="22" spans="1:4">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
     </row>
     <row r="23" spans="1:4" s="5" customFormat="1">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
     </row>
     <row r="24" spans="1:4" s="5" customFormat="1">
-      <c r="A24" s="9"/>
+      <c r="A24" s="11"/>
       <c r="B24" s="6" t="s">
         <v>9</v>
       </c>
@@ -3003,13 +3008,13 @@
       <c r="A25" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="8">
         <v>1.0001660000000001</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="9">
         <v>5.9998040000000001</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="9">
         <v>21.000146999999998</v>
       </c>
     </row>
@@ -3017,13 +3022,13 @@
       <c r="A26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="8">
         <v>1.9998549999999999</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="9">
         <v>16.000032000000001</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="9">
         <v>50.999879999999997</v>
       </c>
     </row>
@@ -3031,13 +3036,13 @@
       <c r="A27" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="8">
         <v>2.0000930000000001</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="9">
         <v>9.0000630000000008</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="9">
         <v>49.999952</v>
       </c>
     </row>
@@ -3045,13 +3050,13 @@
       <c r="A28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="10">
         <v>3.0000209999999998</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="9">
         <v>9.0000630000000008</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="9">
         <v>52.000045999999998</v>
       </c>
     </row>
@@ -3059,13 +3064,13 @@
       <c r="A29" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="8">
         <v>0</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="9">
         <v>2.0000930000000001</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="9">
         <v>6.9999690000000001</v>
       </c>
     </row>
@@ -3073,13 +3078,13 @@
       <c r="A30" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="8">
         <v>0.99992800000000004</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="9">
         <v>3.0000209999999998</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="9">
         <v>17.000198000000001</v>
       </c>
     </row>
@@ -3087,13 +3092,13 @@
       <c r="A31" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="8">
         <v>1.0001660000000001</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="9">
         <v>3.0000209999999998</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="9">
         <v>18.999815000000002</v>
       </c>
     </row>
@@ -3101,36 +3106,36 @@
       <c r="A32" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="8">
         <v>0.99992800000000004</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="9">
         <v>5.9998040000000001</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="9">
         <v>26.999949999999998</v>
       </c>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
     </row>
     <row r="36" spans="1:4">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="9"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="6" t="s">
         <v>9</v>
       </c>
@@ -3145,13 +3150,13 @@
       <c r="A38" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="10">
+      <c r="B38" s="8">
         <v>1016.99996</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="9">
         <v>8335.0000380000001</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D38" s="9">
         <v>65752.000092999995</v>
       </c>
     </row>
@@ -3159,13 +3164,13 @@
       <c r="A39" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B39" s="8">
         <v>511.99984599999999</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="9">
         <v>4105.0000190000001</v>
       </c>
-      <c r="D39" s="11">
+      <c r="D39" s="9">
         <v>32520.999908000002</v>
       </c>
     </row>
@@ -3173,13 +3178,13 @@
       <c r="A40" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="8">
         <v>1082.0000170000001</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C40" s="9">
         <v>8933.9997770000009</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D40" s="9">
         <v>70546.999930999998</v>
       </c>
     </row>
@@ -3187,13 +3192,13 @@
       <c r="A41" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B41" s="10">
         <v>990.00000999999997</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="9">
         <v>8186.0001089999996</v>
       </c>
-      <c r="D41" s="11">
+      <c r="D41" s="9">
         <v>62664.000033999997</v>
       </c>
     </row>
@@ -3201,13 +3206,13 @@
       <c r="A42" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="8">
         <v>336.99989299999999</v>
       </c>
-      <c r="C42" s="11">
+      <c r="C42" s="9">
         <v>2739.000082</v>
       </c>
-      <c r="D42" s="11">
+      <c r="D42" s="9">
         <v>21128.000021</v>
       </c>
     </row>
@@ -3215,13 +3220,13 @@
       <c r="A43" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="8">
         <v>140.00010499999999</v>
       </c>
-      <c r="C43" s="11">
+      <c r="C43" s="9">
         <v>1088.000059</v>
       </c>
-      <c r="D43" s="11">
+      <c r="D43" s="9">
         <v>8697.000027</v>
       </c>
     </row>
@@ -3229,13 +3234,13 @@
       <c r="A44" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="10">
+      <c r="B44" s="8">
         <v>667.00005499999997</v>
       </c>
-      <c r="C44" s="11">
+      <c r="C44" s="9">
         <v>5213.000059</v>
       </c>
-      <c r="D44" s="11">
+      <c r="D44" s="9">
         <v>42406.000137000003</v>
       </c>
     </row>
@@ -3243,36 +3248,36 @@
       <c r="A45" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B45" s="8">
         <v>363.999844</v>
       </c>
-      <c r="C45" s="11">
+      <c r="C45" s="9">
         <v>2821.9997880000001</v>
       </c>
-      <c r="D45" s="11">
+      <c r="D45" s="9">
         <v>22419.999838</v>
       </c>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="9"/>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="9" t="s">
+      <c r="A49" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="9"/>
+      <c r="A50" s="11"/>
       <c r="B50" s="6" t="s">
         <v>9</v>
       </c>
@@ -3287,13 +3292,13 @@
       <c r="A51" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B51" s="10">
+      <c r="B51" s="8">
         <v>1.0001660000000001</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C51" s="9">
         <v>3.999949</v>
       </c>
-      <c r="D51" s="11">
+      <c r="D51" s="9">
         <v>14.000177000000001</v>
       </c>
     </row>
@@ -3301,13 +3306,13 @@
       <c r="A52" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="10">
+      <c r="B52" s="8">
         <v>0.99992800000000004</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="9">
         <v>3.0000209999999998</v>
       </c>
-      <c r="D52" s="11">
+      <c r="D52" s="9">
         <v>13.999938999999999</v>
       </c>
     </row>
@@ -3315,13 +3320,13 @@
       <c r="A53" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B53" s="10">
+      <c r="B53" s="8">
         <v>0</v>
       </c>
-      <c r="C53" s="11">
+      <c r="C53" s="9">
         <v>1.0001660000000001</v>
       </c>
-      <c r="D53" s="11">
+      <c r="D53" s="9">
         <v>4.0001870000000004</v>
       </c>
     </row>
@@ -3329,27 +3334,27 @@
       <c r="A54" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B54" s="12">
+      <c r="B54" s="10">
         <v>0</v>
       </c>
-      <c r="C54" s="11">
+      <c r="C54" s="9">
         <v>0.99992800000000004</v>
       </c>
-      <c r="D54" s="11">
+      <c r="D54" s="9">
         <v>3.999949</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:D36"/>
     <mergeCell ref="A48:D48"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="B49:D49"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:D36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
working on assignment1 report. Think about storage type for mv_mulit. Add conclusion.
</commit_message>
<xml_diff>
--- a/Assignment1/Assignment_1_result_plot_Kazumi.xlsx
+++ b/Assignment1/Assignment_1_result_plot_Kazumi.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="795" windowWidth="24240" windowHeight="13740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1120" yWindow="800" windowWidth="24240" windowHeight="13740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="-O0" sheetId="1" r:id="rId1"/>
     <sheet name="-O3" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -138,7 +138,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -270,16 +270,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -426,19 +426,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>39.590000000000003</c:v>
+                  <c:v>39.59</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>79.180000000000007</c:v>
+                  <c:v>79.18000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>158.36000000000001</c:v>
+                  <c:v>158.36</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>316.72000000000003</c:v>
+                  <c:v>316.72</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>633.44000000000005</c:v>
+                  <c:v>633.4400000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -489,19 +489,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>100.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>200</c:v>
+                  <c:v>200.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>400</c:v>
+                  <c:v>400.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>800</c:v>
+                  <c:v>800.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -552,19 +552,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>60</c:v>
+                  <c:v>60.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>120</c:v>
+                  <c:v>120.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>240</c:v>
+                  <c:v>240.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>480</c:v>
+                  <c:v>480.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>960</c:v>
+                  <c:v>960.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -615,19 +615,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>49</c:v>
+                  <c:v>49.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>98</c:v>
+                  <c:v>98.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>196</c:v>
+                  <c:v>196.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>392</c:v>
+                  <c:v>392.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>784</c:v>
+                  <c:v>784.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -678,19 +678,19 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>45</c:v>
+                  <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90</c:v>
+                  <c:v>90.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>180</c:v>
+                  <c:v>180.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>360</c:v>
+                  <c:v>360.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>720</c:v>
+                  <c:v>720.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -707,11 +707,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="8438912"/>
-        <c:axId val="8440832"/>
+        <c:axId val="2079165720"/>
+        <c:axId val="2113041816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="8438912"/>
+        <c:axId val="2079165720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -738,7 +738,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="8440832"/>
+        <c:crossAx val="2113041816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -746,7 +746,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="8440832"/>
+        <c:axId val="2113041816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -775,7 +775,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="8438912"/>
+        <c:crossAx val="2079165720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -790,7 +790,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -842,9 +842,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.4719474168293002E-2"/>
-          <c:y val="3.3810143042912903E-2"/>
-          <c:w val="0.61166038098697595"/>
+          <c:x val="0.094719474168293"/>
+          <c:y val="0.0338101430429129"/>
+          <c:w val="0.611660380986976"/>
           <c:h val="0.852553372310906"/>
         </c:manualLayout>
       </c:layout>
@@ -896,13 +896,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.0001660000000001</c:v>
+                  <c:v>1.000166</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9998040000000001</c:v>
+                  <c:v>5.999804</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.000146999999998</c:v>
+                  <c:v>21.000147</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -954,13 +954,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.9998549999999999</c:v>
+                  <c:v>1.999855</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.000032000000001</c:v>
+                  <c:v>16.000032</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.999879999999997</c:v>
+                  <c:v>50.99988</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1012,10 +1012,10 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2.0000930000000001</c:v>
+                  <c:v>2.000093</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0000630000000008</c:v>
+                  <c:v>9.000063000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>49.999952</c:v>
@@ -1070,13 +1070,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.0000209999999998</c:v>
+                  <c:v>3.000021</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.0000630000000008</c:v>
+                  <c:v>9.000063000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.000045999999998</c:v>
+                  <c:v>52.000046</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1128,13 +1128,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0000930000000001</c:v>
+                  <c:v>2.000093</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.9999690000000001</c:v>
+                  <c:v>6.999969</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1186,13 +1186,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.99992800000000004</c:v>
+                  <c:v>0.999928</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0000209999999998</c:v>
+                  <c:v>3.000021</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.000198000000001</c:v>
+                  <c:v>17.000198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1244,13 +1244,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.0001660000000001</c:v>
+                  <c:v>1.000166</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0000209999999998</c:v>
+                  <c:v>3.000021</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18.999815000000002</c:v>
+                  <c:v>18.999815</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1302,13 +1302,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.99992800000000004</c:v>
+                  <c:v>0.999928</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.9998040000000001</c:v>
+                  <c:v>5.999804</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.999949999999998</c:v>
+                  <c:v>26.99995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1325,11 +1325,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="89159168"/>
-        <c:axId val="89160704"/>
+        <c:axId val="2100954136"/>
+        <c:axId val="2100200280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89159168"/>
+        <c:axId val="2100954136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1338,7 +1338,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89160704"/>
+        <c:crossAx val="2100200280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1346,7 +1346,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89160704"/>
+        <c:axId val="2100200280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1376,7 +1376,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89159168"/>
+        <c:crossAx val="2100954136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1387,10 +1387,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.75033921302577999"/>
-          <c:y val="0.30700450905175303"/>
+          <c:x val="0.75033921302578"/>
+          <c:y val="0.307004509051753"/>
           <c:w val="0.238805970149254"/>
-          <c:h val="0.42897022487573699"/>
+          <c:h val="0.428970224875737"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1401,7 +1401,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1454,10 +1454,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.5015898343103604E-2"/>
-          <c:y val="3.2622333751568401E-2"/>
-          <c:w val="0.74966954571207201"/>
-          <c:h val="0.85773342949446196"/>
+          <c:x val="0.0650158983431036"/>
+          <c:y val="0.0326223337515684"/>
+          <c:w val="0.749669545712072"/>
+          <c:h val="0.857733429494462"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1511,10 +1511,10 @@
                   <c:v>1016.99996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8335.0000380000001</c:v>
+                  <c:v>8335.000038</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65752.000092999995</c:v>
+                  <c:v>65752.000093</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1566,13 +1566,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>511.99984599999999</c:v>
+                  <c:v>511.999846</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4105.0000190000001</c:v>
+                  <c:v>4105.000019</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32520.999908000002</c:v>
+                  <c:v>32520.999908</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1624,13 +1624,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1082.0000170000001</c:v>
+                  <c:v>1082.000017</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8933.9997770000009</c:v>
+                  <c:v>8933.999777</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>70546.999930999998</c:v>
+                  <c:v>70546.999931</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1682,13 +1682,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>990.00000999999997</c:v>
+                  <c:v>990.00001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8186.0001089999996</c:v>
+                  <c:v>8186.000109</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>62664.000033999997</c:v>
+                  <c:v>62664.000034</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1740,7 +1740,7 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>336.99989299999999</c:v>
+                  <c:v>336.999893</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2739.000082</c:v>
@@ -1798,7 +1798,7 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>140.00010499999999</c:v>
+                  <c:v>140.000105</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1088.000059</c:v>
@@ -1856,13 +1856,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>667.00005499999997</c:v>
+                  <c:v>667.000055</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5213.000059</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42406.000137000003</c:v>
+                  <c:v>42406.000137</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1917,7 +1917,7 @@
                   <c:v>363.999844</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2821.9997880000001</c:v>
+                  <c:v>2821.999788</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>22419.999838</c:v>
@@ -1937,11 +1937,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="89871488"/>
-        <c:axId val="89873024"/>
+        <c:axId val="2078355592"/>
+        <c:axId val="-2133442744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89871488"/>
+        <c:axId val="2078355592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1950,7 +1950,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89873024"/>
+        <c:crossAx val="-2133442744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1958,7 +1958,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89873024"/>
+        <c:axId val="-2133442744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1969,7 +1969,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89871488"/>
+        <c:crossAx val="2078355592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1985,7 +1985,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2038,9 +2038,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.2010961865060998E-2"/>
-          <c:y val="3.2459425717852701E-2"/>
-          <c:w val="0.77757019343170297"/>
+          <c:x val="0.062010961865061"/>
+          <c:y val="0.0324594257178527"/>
+          <c:w val="0.777570193431703"/>
           <c:h val="0.858443874290995"/>
         </c:manualLayout>
       </c:layout>
@@ -2092,13 +2092,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.0001660000000001</c:v>
+                  <c:v>1.000166</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.999949</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.000177000000001</c:v>
+                  <c:v>14.000177</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2150,13 +2150,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.99992800000000004</c:v>
+                  <c:v>0.999928</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0000209999999998</c:v>
+                  <c:v>3.000021</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.999938999999999</c:v>
+                  <c:v>13.999939</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2208,13 +2208,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0001660000000001</c:v>
+                  <c:v>1.000166</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.0001870000000004</c:v>
+                  <c:v>4.000187</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2266,10 +2266,10 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99992800000000004</c:v>
+                  <c:v>0.999928</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3.999949</c:v>
@@ -2289,11 +2289,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="89900160"/>
-        <c:axId val="89901696"/>
+        <c:axId val="2112065384"/>
+        <c:axId val="2115736776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89900160"/>
+        <c:axId val="2112065384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2302,7 +2302,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89901696"/>
+        <c:crossAx val="2115736776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2310,7 +2310,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89901696"/>
+        <c:axId val="2115736776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2321,7 +2321,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89900160"/>
+        <c:crossAx val="2112065384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2337,7 +2337,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2801,21 +2801,21 @@
       <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:8">
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:8">
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:8">
       <c r="C25" t="s">
         <v>4</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>633.44000000000005</v>
       </c>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:8">
       <c r="C26" t="s">
         <v>3</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:8">
       <c r="C27" t="s">
         <v>2</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:8">
       <c r="C28" t="s">
         <v>1</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:8">
       <c r="C29" t="s">
         <v>0</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:8">
       <c r="D30" t="s">
         <v>5</v>
       </c>
@@ -2966,39 +2966,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A22:D54"/>
+  <dimension ref="A22:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="50" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51:D54"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+    <row r="22" spans="1:5">
+      <c r="A22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+    </row>
+    <row r="23" spans="1:5" s="5" customFormat="1">
+      <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="9"/>
-    </row>
-    <row r="24" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:5" s="5" customFormat="1">
+      <c r="A24" s="11"/>
       <c r="B24" s="6" t="s">
         <v>9</v>
       </c>
@@ -3009,138 +3009,154 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="8">
         <v>1.0001660000000001</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="9">
         <v>5.9998040000000001</v>
       </c>
-      <c r="D25" s="11">
+      <c r="D25" s="9">
         <v>21.000146999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="8">
         <v>1.9998549999999999</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="9">
         <v>16.000032000000001</v>
       </c>
-      <c r="D26" s="11">
+      <c r="D26" s="9">
         <v>50.999879999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="10">
+      <c r="B27" s="8">
         <v>2.0000930000000001</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="9">
         <v>9.0000630000000008</v>
       </c>
-      <c r="D27" s="11">
+      <c r="D27" s="9">
         <v>49.999952</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="12">
+      <c r="B28" s="10">
         <v>3.0000209999999998</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="9">
         <v>9.0000630000000008</v>
       </c>
-      <c r="D28" s="11">
+      <c r="D28" s="9">
         <v>52.000045999999998</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="10">
+      <c r="B29" s="8">
         <v>0</v>
       </c>
-      <c r="C29" s="11">
+      <c r="C29" s="9">
         <v>2.0000930000000001</v>
       </c>
-      <c r="D29" s="11">
+      <c r="D29" s="9">
         <v>6.9999690000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <f>D25/D29</f>
+        <v>3.0000342858661226</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="10">
+      <c r="B30" s="8">
         <v>0.99992800000000004</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="9">
         <v>3.0000209999999998</v>
       </c>
-      <c r="D30" s="11">
+      <c r="D30" s="9">
         <v>17.000198000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <f t="shared" ref="E30:E32" si="0">D26/D30</f>
+        <v>2.9999580004891704</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="10">
+      <c r="B31" s="8">
         <v>1.0001660000000001</v>
       </c>
-      <c r="C31" s="11">
+      <c r="C31" s="9">
         <v>3.0000209999999998</v>
       </c>
-      <c r="D31" s="11">
+      <c r="D31" s="9">
         <v>18.999815000000002</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>2.6316020445462232</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="10">
+      <c r="B32" s="8">
         <v>0.99992800000000004</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="9">
         <v>5.9998040000000001</v>
       </c>
-      <c r="D32" s="11">
+      <c r="D32" s="9">
         <v>26.999949999999998</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>1.9259311961688819</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="B35" s="11"/>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="11"/>
       <c r="B37" s="6" t="s">
         <v>9</v>
       </c>
@@ -3151,138 +3167,154 @@
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="10">
+      <c r="B38" s="8">
         <v>1016.99996</v>
       </c>
-      <c r="C38" s="11">
+      <c r="C38" s="9">
         <v>8335.0000380000001</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D38" s="9">
         <v>65752.000092999995</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B39" s="8">
         <v>511.99984599999999</v>
       </c>
-      <c r="C39" s="11">
+      <c r="C39" s="9">
         <v>4105.0000190000001</v>
       </c>
-      <c r="D39" s="11">
+      <c r="D39" s="9">
         <v>32520.999908000002</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="8">
         <v>1082.0000170000001</v>
       </c>
-      <c r="C40" s="11">
+      <c r="C40" s="9">
         <v>8933.9997770000009</v>
       </c>
-      <c r="D40" s="11">
+      <c r="D40" s="9">
         <v>70546.999930999998</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B41" s="10">
         <v>990.00000999999997</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="9">
         <v>8186.0001089999996</v>
       </c>
-      <c r="D41" s="11">
+      <c r="D41" s="9">
         <v>62664.000033999997</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="8">
         <v>336.99989299999999</v>
       </c>
-      <c r="C42" s="11">
+      <c r="C42" s="9">
         <v>2739.000082</v>
       </c>
-      <c r="D42" s="11">
+      <c r="D42" s="9">
         <v>21128.000021</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <f>D38/D42</f>
+        <v>3.1120787593547115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="10">
+      <c r="B43" s="8">
         <v>140.00010499999999</v>
       </c>
-      <c r="C43" s="11">
+      <c r="C43" s="9">
         <v>1088.000059</v>
       </c>
-      <c r="D43" s="11">
+      <c r="D43" s="9">
         <v>8697.000027</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <f t="shared" ref="E43:E45" si="1">D39/D43</f>
+        <v>3.7393353808253358</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="10">
+      <c r="B44" s="8">
         <v>667.00005499999997</v>
       </c>
-      <c r="C44" s="11">
+      <c r="C44" s="9">
         <v>5213.000059</v>
       </c>
-      <c r="D44" s="11">
+      <c r="D44" s="9">
         <v>42406.000137000003</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>1.6636089162638676</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B45" s="10">
+      <c r="B45" s="8">
         <v>363.999844</v>
       </c>
-      <c r="C45" s="11">
+      <c r="C45" s="9">
         <v>2821.9997880000001</v>
       </c>
-      <c r="D45" s="11">
+      <c r="D45" s="9">
         <v>22419.999838</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>2.7950044820156434</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="9"/>
-      <c r="D49" s="9"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="8"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="12"/>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="11"/>
       <c r="B50" s="6" t="s">
         <v>9</v>
       </c>
@@ -3293,60 +3325,68 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5">
       <c r="A51" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B51" s="10">
+      <c r="B51" s="8">
         <v>1.0001660000000001</v>
       </c>
-      <c r="C51" s="11">
+      <c r="C51" s="9">
         <v>3.999949</v>
       </c>
-      <c r="D51" s="11">
+      <c r="D51" s="9">
         <v>14.000177000000001</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5">
       <c r="A52" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="10">
+      <c r="B52" s="8">
         <v>0.99992800000000004</v>
       </c>
-      <c r="C52" s="11">
+      <c r="C52" s="9">
         <v>3.0000209999999998</v>
       </c>
-      <c r="D52" s="11">
+      <c r="D52" s="9">
         <v>13.999938999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5">
       <c r="A53" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B53" s="10">
+      <c r="B53" s="8">
         <v>0</v>
       </c>
-      <c r="C53" s="11">
+      <c r="C53" s="9">
         <v>1.0001660000000001</v>
       </c>
-      <c r="D53" s="11">
+      <c r="D53" s="9">
         <v>4.0001870000000004</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <f>D51/D53</f>
+        <v>3.4998806305805203</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B54" s="12">
+      <c r="B54" s="10">
         <v>0</v>
       </c>
-      <c r="C54" s="11">
+      <c r="C54" s="9">
         <v>0.99992800000000004</v>
       </c>
-      <c r="D54" s="11">
+      <c r="D54" s="9">
         <v>3.999949</v>
+      </c>
+      <c r="E54">
+        <f>D52/D54</f>
+        <v>3.500029375374536</v>
       </c>
     </row>
   </sheetData>
@@ -3362,8 +3402,8 @@
     <mergeCell ref="A48:D48"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Completed assignment 1 report. Now Review.
</commit_message>
<xml_diff>
--- a/Assignment1/Assignment_1_result_plot_Kazumi.xlsx
+++ b/Assignment1/Assignment_1_result_plot_Kazumi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="800" windowWidth="24240" windowHeight="13740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="-O0" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>base</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>mv_multiplication(col) -O3</t>
+  </si>
+  <si>
+    <t>O0 vs O3</t>
+  </si>
+  <si>
+    <t>Memory access</t>
   </si>
 </sst>
 </file>
@@ -707,11 +713,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2079165720"/>
-        <c:axId val="2113041816"/>
+        <c:axId val="-2132208280"/>
+        <c:axId val="-2131929112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2079165720"/>
+        <c:axId val="-2132208280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -738,7 +744,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2113041816"/>
+        <c:crossAx val="-2131929112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -746,7 +752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2113041816"/>
+        <c:axId val="-2131929112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -775,7 +781,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079165720"/>
+        <c:crossAx val="-2132208280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -856,7 +862,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$25</c:f>
+              <c:f>'-O3'!$B$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -867,7 +873,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$22:$D$24</c:f>
+              <c:f>'-O3'!$C$22:$E$24</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -891,7 +897,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$25:$D$25</c:f>
+              <c:f>'-O3'!$C$25:$E$25</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -914,7 +920,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$26</c:f>
+              <c:f>'-O3'!$B$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -925,7 +931,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$22:$D$24</c:f>
+              <c:f>'-O3'!$C$22:$E$24</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -949,7 +955,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$26:$D$26</c:f>
+              <c:f>'-O3'!$C$26:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -972,7 +978,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$27</c:f>
+              <c:f>'-O3'!$B$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -983,7 +989,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$22:$D$24</c:f>
+              <c:f>'-O3'!$C$22:$E$24</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -1007,7 +1013,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$27:$D$27</c:f>
+              <c:f>'-O3'!$C$27:$E$27</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1030,7 +1036,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$28</c:f>
+              <c:f>'-O3'!$B$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1041,7 +1047,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$22:$D$24</c:f>
+              <c:f>'-O3'!$C$22:$E$24</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -1065,7 +1071,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$28:$D$28</c:f>
+              <c:f>'-O3'!$C$28:$E$28</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1088,7 +1094,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$29</c:f>
+              <c:f>'-O3'!$B$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1099,7 +1105,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$22:$D$24</c:f>
+              <c:f>'-O3'!$C$22:$E$24</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -1123,7 +1129,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$29:$D$29</c:f>
+              <c:f>'-O3'!$C$29:$E$29</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1146,7 +1152,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$30</c:f>
+              <c:f>'-O3'!$B$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1157,7 +1163,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$22:$D$24</c:f>
+              <c:f>'-O3'!$C$22:$E$24</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -1181,7 +1187,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$30:$D$30</c:f>
+              <c:f>'-O3'!$C$30:$E$30</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1204,7 +1210,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$31</c:f>
+              <c:f>'-O3'!$B$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1215,7 +1221,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$22:$D$24</c:f>
+              <c:f>'-O3'!$C$22:$E$24</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -1239,7 +1245,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$31:$D$31</c:f>
+              <c:f>'-O3'!$C$31:$E$31</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1262,7 +1268,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$32</c:f>
+              <c:f>'-O3'!$B$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1273,7 +1279,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$22:$D$24</c:f>
+              <c:f>'-O3'!$C$22:$E$24</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -1297,7 +1303,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$32:$D$32</c:f>
+              <c:f>'-O3'!$C$32:$E$32</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1325,11 +1331,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2100954136"/>
-        <c:axId val="2100200280"/>
+        <c:axId val="-2131858344"/>
+        <c:axId val="-2131855368"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2100954136"/>
+        <c:axId val="-2131858344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1338,7 +1344,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100200280"/>
+        <c:crossAx val="-2131855368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1346,7 +1352,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2100200280"/>
+        <c:axId val="-2131855368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1376,7 +1382,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2100954136"/>
+        <c:crossAx val="-2131858344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1468,7 +1474,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$38</c:f>
+              <c:f>'-O3'!$B$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1479,7 +1485,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$36:$D$37</c:f>
+              <c:f>'-O3'!$C$36:$E$37</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -1503,7 +1509,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$38:$D$38</c:f>
+              <c:f>'-O3'!$C$38:$E$38</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1526,7 +1532,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$39</c:f>
+              <c:f>'-O3'!$B$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1537,7 +1543,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$36:$D$37</c:f>
+              <c:f>'-O3'!$C$36:$E$37</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -1561,7 +1567,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$39:$D$39</c:f>
+              <c:f>'-O3'!$C$39:$E$39</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1584,7 +1590,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$40</c:f>
+              <c:f>'-O3'!$B$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1595,7 +1601,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$36:$D$37</c:f>
+              <c:f>'-O3'!$C$36:$E$37</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -1619,7 +1625,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$40:$D$40</c:f>
+              <c:f>'-O3'!$C$40:$E$40</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1642,7 +1648,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$41</c:f>
+              <c:f>'-O3'!$B$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1653,7 +1659,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$36:$D$37</c:f>
+              <c:f>'-O3'!$C$36:$E$37</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -1677,7 +1683,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$41:$D$41</c:f>
+              <c:f>'-O3'!$C$41:$E$41</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1700,7 +1706,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$42</c:f>
+              <c:f>'-O3'!$B$42</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1711,7 +1717,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$36:$D$37</c:f>
+              <c:f>'-O3'!$C$36:$E$37</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -1735,7 +1741,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$42:$D$42</c:f>
+              <c:f>'-O3'!$C$42:$E$42</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1758,7 +1764,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$43</c:f>
+              <c:f>'-O3'!$B$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1769,7 +1775,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$36:$D$37</c:f>
+              <c:f>'-O3'!$C$36:$E$37</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -1793,7 +1799,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$43:$D$43</c:f>
+              <c:f>'-O3'!$C$43:$E$43</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1816,7 +1822,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$44</c:f>
+              <c:f>'-O3'!$B$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1827,7 +1833,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$36:$D$37</c:f>
+              <c:f>'-O3'!$C$36:$E$37</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -1851,7 +1857,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$44:$D$44</c:f>
+              <c:f>'-O3'!$C$44:$E$44</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1874,7 +1880,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$45</c:f>
+              <c:f>'-O3'!$B$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1885,7 +1891,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$36:$D$37</c:f>
+              <c:f>'-O3'!$C$36:$E$37</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -1909,7 +1915,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$45:$D$45</c:f>
+              <c:f>'-O3'!$C$45:$E$45</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1937,11 +1943,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2078355592"/>
-        <c:axId val="-2133442744"/>
+        <c:axId val="-2131799048"/>
+        <c:axId val="-2131796072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2078355592"/>
+        <c:axId val="-2131799048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1950,7 +1956,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133442744"/>
+        <c:crossAx val="-2131796072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1958,7 +1964,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133442744"/>
+        <c:axId val="-2131796072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1969,7 +1975,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078355592"/>
+        <c:crossAx val="-2131799048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2052,7 +2058,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$51</c:f>
+              <c:f>'-O3'!$B$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2063,7 +2069,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$49:$D$50</c:f>
+              <c:f>'-O3'!$C$49:$E$50</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -2087,18 +2093,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$51:$D$51</c:f>
+              <c:f>'-O3'!$C$51:$E$51</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1.000166</c:v>
+                  <c:v>0.999928</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3.999949</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14.000177</c:v>
+                  <c:v>13.000011</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2110,7 +2116,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$52</c:f>
+              <c:f>'-O3'!$B$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2121,7 +2127,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$49:$D$50</c:f>
+              <c:f>'-O3'!$C$49:$E$50</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -2145,18 +2151,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$52:$D$52</c:f>
+              <c:f>'-O3'!$C$52:$E$52</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.999928</c:v>
+                  <c:v>2.000093</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.000021</c:v>
+                  <c:v>6.000042</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.999939</c:v>
+                  <c:v>26.99995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2168,7 +2174,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$53</c:f>
+              <c:f>'-O3'!$B$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2179,7 +2185,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$49:$D$50</c:f>
+              <c:f>'-O3'!$C$49:$E$50</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -2203,7 +2209,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$53:$D$53</c:f>
+              <c:f>'-O3'!$C$53:$E$53</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2211,10 +2217,10 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.000166</c:v>
+                  <c:v>0.999928</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.000187</c:v>
+                  <c:v>4.999876</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2226,7 +2232,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'-O3'!$A$54</c:f>
+              <c:f>'-O3'!$B$54</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2237,7 +2243,7 @@
           </c:tx>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'-O3'!$B$49:$D$50</c:f>
+              <c:f>'-O3'!$C$49:$E$50</c:f>
               <c:multiLvlStrCache>
                 <c:ptCount val="3"/>
                 <c:lvl>
@@ -2261,18 +2267,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'-O3'!$B$54:$D$54</c:f>
+              <c:f>'-O3'!$C$54:$E$54</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.999928</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.999928</c:v>
+                  <c:v>3.000021</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.999949</c:v>
+                  <c:v>12.000084</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2289,11 +2295,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2112065384"/>
-        <c:axId val="2115736776"/>
+        <c:axId val="2121627368"/>
+        <c:axId val="2121630488"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2112065384"/>
+        <c:axId val="2121627368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2302,7 +2308,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115736776"/>
+        <c:crossAx val="2121630488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2310,7 +2316,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115736776"/>
+        <c:axId val="2121630488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2321,7 +2327,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2112065384"/>
+        <c:crossAx val="2121627368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2382,16 +2388,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>635000</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2412,16 +2418,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2442,15 +2448,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>139700</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>146050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>93</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2966,440 +2972,469 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A22:E54"/>
+  <dimension ref="B21:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="22" spans="1:5">
-      <c r="A22" s="11" t="s">
+    <row r="21" spans="2:9">
+      <c r="F21" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="11"/>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
-    </row>
-    <row r="23" spans="1:5" s="5" customFormat="1">
-      <c r="A23" s="11" t="s">
+      <c r="E22" s="11"/>
+      <c r="G22">
+        <v>512</v>
+      </c>
+      <c r="H22">
+        <v>1024</v>
+      </c>
+      <c r="I22">
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" s="5" customFormat="1">
+      <c r="B23" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="C23" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="12"/>
       <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="1:5" s="5" customFormat="1">
-      <c r="A24" s="11"/>
-      <c r="B24" s="6" t="s">
+      <c r="E23" s="12"/>
+    </row>
+    <row r="24" spans="2:9" s="5" customFormat="1">
+      <c r="B24" s="11"/>
+      <c r="C24" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="D24" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="E24" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="7" t="s">
+    <row r="25" spans="2:9">
+      <c r="B25" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="8">
+      <c r="C25" s="8">
         <v>1.0001660000000001</v>
       </c>
-      <c r="C25" s="9">
+      <c r="D25" s="9">
         <v>5.9998040000000001</v>
       </c>
-      <c r="D25" s="9">
+      <c r="E25" s="9">
         <v>21.000146999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="7" t="s">
+    <row r="26" spans="2:9">
+      <c r="B26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="8">
+      <c r="C26" s="8">
         <v>1.9998549999999999</v>
       </c>
-      <c r="C26" s="9">
+      <c r="D26" s="9">
         <v>16.000032000000001</v>
       </c>
-      <c r="D26" s="9">
+      <c r="E26" s="9">
         <v>50.999879999999997</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="7" t="s">
+      <c r="G26">
+        <f>$C$25/C26</f>
+        <v>0.50011925864625195</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="8">
+      <c r="C27" s="8">
         <v>2.0000930000000001</v>
       </c>
-      <c r="C27" s="9">
+      <c r="D27" s="9">
         <v>9.0000630000000008</v>
       </c>
-      <c r="D27" s="9">
+      <c r="E27" s="9">
         <v>49.999952</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="7" t="s">
+      <c r="G27">
+        <f t="shared" ref="G27:G28" si="0">$C$25/C27</f>
+        <v>0.50005974722175417</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="10">
+      <c r="C28" s="10">
         <v>3.0000209999999998</v>
       </c>
-      <c r="C28" s="9">
+      <c r="D28" s="9">
         <v>9.0000630000000008</v>
       </c>
-      <c r="D28" s="9">
+      <c r="E28" s="9">
         <v>52.000045999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="7" t="s">
+      <c r="G28">
+        <f t="shared" si="0"/>
+        <v>0.333386332962336</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="8">
+      <c r="C29" s="8">
         <v>0</v>
       </c>
-      <c r="C29" s="9">
+      <c r="D29" s="9">
         <v>2.0000930000000001</v>
       </c>
-      <c r="D29" s="9">
+      <c r="E29" s="9">
         <v>6.9999690000000001</v>
       </c>
-      <c r="E29">
-        <f>D25/D29</f>
+      <c r="F29">
+        <f>E25/E29</f>
         <v>3.0000342858661226</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="7" t="s">
+    <row r="30" spans="2:9">
+      <c r="B30" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="8">
+      <c r="C30" s="8">
         <v>0.99992800000000004</v>
       </c>
-      <c r="C30" s="9">
+      <c r="D30" s="9">
         <v>3.0000209999999998</v>
       </c>
-      <c r="D30" s="9">
+      <c r="E30" s="9">
         <v>17.000198000000001</v>
       </c>
-      <c r="E30">
-        <f t="shared" ref="E30:E32" si="0">D26/D30</f>
+      <c r="F30">
+        <f t="shared" ref="F30:F32" si="1">E26/E30</f>
         <v>2.9999580004891704</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="7" t="s">
+    <row r="31" spans="2:9">
+      <c r="B31" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="8">
+      <c r="C31" s="8">
         <v>1.0001660000000001</v>
       </c>
-      <c r="C31" s="9">
+      <c r="D31" s="9">
         <v>3.0000209999999998</v>
       </c>
-      <c r="D31" s="9">
+      <c r="E31" s="9">
         <v>18.999815000000002</v>
       </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
+      <c r="F31">
+        <f t="shared" si="1"/>
         <v>2.6316020445462232</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="7" t="s">
+    <row r="32" spans="2:9">
+      <c r="B32" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="8">
+      <c r="C32" s="8">
         <v>0.99992800000000004</v>
       </c>
-      <c r="C32" s="9">
+      <c r="D32" s="9">
         <v>5.9998040000000001</v>
       </c>
-      <c r="D32" s="9">
+      <c r="E32" s="9">
         <v>26.999949999999998</v>
       </c>
-      <c r="E32">
-        <f t="shared" si="0"/>
+      <c r="F32">
+        <f t="shared" si="1"/>
         <v>1.9259311961688819</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="11" t="s">
+    <row r="35" spans="2:6">
+      <c r="B35" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="11"/>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="11" t="s">
+      <c r="E35" s="11"/>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="C36" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="12"/>
       <c r="D36" s="12"/>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="11"/>
-      <c r="B37" s="6" t="s">
+      <c r="E36" s="12"/>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="11"/>
+      <c r="C37" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="D37" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="6" t="s">
+      <c r="E37" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="7" t="s">
+    <row r="38" spans="2:6">
+      <c r="B38" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="8">
+      <c r="C38" s="8">
         <v>1016.99996</v>
       </c>
-      <c r="C38" s="9">
+      <c r="D38" s="9">
         <v>8335.0000380000001</v>
       </c>
-      <c r="D38" s="9">
+      <c r="E38" s="9">
         <v>65752.000092999995</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="7" t="s">
+    <row r="39" spans="2:6">
+      <c r="B39" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="8">
+      <c r="C39" s="8">
         <v>511.99984599999999</v>
       </c>
-      <c r="C39" s="9">
+      <c r="D39" s="9">
         <v>4105.0000190000001</v>
       </c>
-      <c r="D39" s="9">
+      <c r="E39" s="9">
         <v>32520.999908000002</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="7" t="s">
+    <row r="40" spans="2:6">
+      <c r="B40" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B40" s="8">
+      <c r="C40" s="8">
         <v>1082.0000170000001</v>
       </c>
-      <c r="C40" s="9">
+      <c r="D40" s="9">
         <v>8933.9997770000009</v>
       </c>
-      <c r="D40" s="9">
+      <c r="E40" s="9">
         <v>70546.999930999998</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="7" t="s">
+    <row r="41" spans="2:6">
+      <c r="B41" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B41" s="10">
+      <c r="C41" s="10">
         <v>990.00000999999997</v>
       </c>
-      <c r="C41" s="9">
+      <c r="D41" s="9">
         <v>8186.0001089999996</v>
       </c>
-      <c r="D41" s="9">
+      <c r="E41" s="9">
         <v>62664.000033999997</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="7" t="s">
+    <row r="42" spans="2:6">
+      <c r="B42" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B42" s="8">
+      <c r="C42" s="8">
         <v>336.99989299999999</v>
       </c>
-      <c r="C42" s="9">
+      <c r="D42" s="9">
         <v>2739.000082</v>
       </c>
-      <c r="D42" s="9">
+      <c r="E42" s="9">
         <v>21128.000021</v>
       </c>
-      <c r="E42">
-        <f>D38/D42</f>
+      <c r="F42">
+        <f>E38/E42</f>
         <v>3.1120787593547115</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="7" t="s">
+    <row r="43" spans="2:6">
+      <c r="B43" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B43" s="8">
+      <c r="C43" s="8">
         <v>140.00010499999999</v>
       </c>
-      <c r="C43" s="9">
+      <c r="D43" s="9">
         <v>1088.000059</v>
       </c>
-      <c r="D43" s="9">
+      <c r="E43" s="9">
         <v>8697.000027</v>
       </c>
-      <c r="E43">
-        <f t="shared" ref="E43:E45" si="1">D39/D43</f>
+      <c r="F43">
+        <f t="shared" ref="F43:F45" si="2">E39/E43</f>
         <v>3.7393353808253358</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="7" t="s">
+    <row r="44" spans="2:6">
+      <c r="B44" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="8">
+      <c r="C44" s="8">
         <v>667.00005499999997</v>
       </c>
-      <c r="C44" s="9">
+      <c r="D44" s="9">
         <v>5213.000059</v>
       </c>
-      <c r="D44" s="9">
+      <c r="E44" s="9">
         <v>42406.000137000003</v>
       </c>
-      <c r="E44">
-        <f t="shared" si="1"/>
+      <c r="F44">
+        <f t="shared" si="2"/>
         <v>1.6636089162638676</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="7" t="s">
+    <row r="45" spans="2:6">
+      <c r="B45" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B45" s="8">
+      <c r="C45" s="8">
         <v>363.999844</v>
       </c>
-      <c r="C45" s="9">
+      <c r="D45" s="9">
         <v>2821.9997880000001</v>
       </c>
-      <c r="D45" s="9">
+      <c r="E45" s="9">
         <v>22419.999838</v>
       </c>
-      <c r="E45">
-        <f t="shared" si="1"/>
+      <c r="F45">
+        <f t="shared" si="2"/>
         <v>2.7950044820156434</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="11" t="s">
+    <row r="48" spans="2:6">
+      <c r="B48" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="11"/>
       <c r="C48" s="11"/>
       <c r="D48" s="11"/>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="11" t="s">
+      <c r="E48" s="11"/>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="B49" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="C49" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="12"/>
       <c r="D49" s="12"/>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="11"/>
-      <c r="B50" s="6" t="s">
+      <c r="E49" s="12"/>
+    </row>
+    <row r="50" spans="2:6">
+      <c r="B50" s="11"/>
+      <c r="C50" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="D50" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D50" s="6" t="s">
+      <c r="E50" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="7" t="s">
+    <row r="51" spans="2:6">
+      <c r="B51" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B51" s="8">
-        <v>1.0001660000000001</v>
-      </c>
-      <c r="C51" s="9">
+      <c r="C51" s="8">
+        <v>0.99992800000000004</v>
+      </c>
+      <c r="D51" s="9">
         <v>3.999949</v>
       </c>
-      <c r="D51" s="9">
-        <v>14.000177000000001</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="7" t="s">
+      <c r="E51" s="9">
+        <v>13.000011000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="B52" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B52" s="8">
+      <c r="C52" s="8">
+        <v>2.0000930000000001</v>
+      </c>
+      <c r="D52" s="9">
+        <v>6.0000419999999997</v>
+      </c>
+      <c r="E52" s="9">
+        <v>26.999949999999998</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="B53" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" s="8">
+        <v>0</v>
+      </c>
+      <c r="D53" s="9">
         <v>0.99992800000000004</v>
       </c>
-      <c r="C52" s="9">
+      <c r="E53" s="9">
+        <v>4.9998760000000004</v>
+      </c>
+      <c r="F53">
+        <f>E51/E53</f>
+        <v>2.600066681653705</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="10">
+        <v>0.99992800000000004</v>
+      </c>
+      <c r="D54" s="9">
         <v>3.0000209999999998</v>
       </c>
-      <c r="D52" s="9">
-        <v>13.999938999999999</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B53" s="8">
-        <v>0</v>
-      </c>
-      <c r="C53" s="9">
-        <v>1.0001660000000001</v>
-      </c>
-      <c r="D53" s="9">
-        <v>4.0001870000000004</v>
-      </c>
-      <c r="E53">
-        <f>D51/D53</f>
-        <v>3.4998806305805203</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B54" s="10">
-        <v>0</v>
-      </c>
-      <c r="C54" s="9">
-        <v>0.99992800000000004</v>
-      </c>
-      <c r="D54" s="9">
-        <v>3.999949</v>
-      </c>
-      <c r="E54">
-        <f>D52/D54</f>
-        <v>3.500029375374536</v>
+      <c r="E54" s="9">
+        <v>12.000083999999999</v>
+      </c>
+      <c r="F54">
+        <f>E52/E54</f>
+        <v>2.249980083472749</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="B48:E48"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>